<commit_message>
[Md Ahsanullah] Add: financial statement script for VK global
</commit_message>
<xml_diff>
--- a/Excel output files/Company ACRA output.xlsx
+++ b/Excel output files/Company ACRA output.xlsx
@@ -120,7 +120,40 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="21">
+  <x:cellStyleXfs count="32">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>